<commit_message>
added reruns to excel file
</commit_message>
<xml_diff>
--- a/benchmark/NAS-PBv3.3.1 P2C Benchmarking (default scheduler).xlsx
+++ b/benchmark/NAS-PBv3.3.1 P2C Benchmarking (default scheduler).xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="BT" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,8 @@
     <sheet name="SP" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="GNUPlot-Time-Class-A" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="GNUPlot-Time-Class-B" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="GNUPlot-Time-Class-A-Rerun" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="GNUPlot-Time-Class-B-Rerun" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="27">
   <si>
     <t xml:space="preserve">BT</t>
   </si>
@@ -241,9 +243,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,10 +401,13 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -562,8 +567,175 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>80.95</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>42.11</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>43.08</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>46.37</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>147.76</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>80.85</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>40.47</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>20.37</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>12.31</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>6.12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>81.29</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>71.63</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>51.86</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>34.66</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>4.56</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>157.25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>267.3</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>137.49</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>101.38</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>75.05</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>276.44</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>8.89</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>5.52</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>2.55</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -596,59 +768,49 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>80.95</v>
+        <v>1.18</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>42.11</v>
+        <v>1.05</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>43.08</v>
+        <v>1.34</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>46.37</v>
+        <v>1.46</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>147.76</v>
+        <v>78.66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>80.85</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>40.47</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>20.37</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>12.31</v>
-      </c>
-      <c r="F3" s="3" t="n">
-        <v>6.12</v>
-      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>26</v>
+      <c r="B4" s="3" t="n">
+        <v>4.81</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>81.29</v>
+        <v>4.97</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>71.63</v>
+        <v>6.03</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>51.86</v>
+        <v>4.49</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>34.66</v>
+        <v>9.21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,19 +818,19 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>2.84</v>
+        <v>0.64</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>4.56</v>
+        <v>1.14</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>3.59</v>
+        <v>0.91</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>3.76</v>
+        <v>0.89</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>157.25</v>
+        <v>6.76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,40 +838,177 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>267.3</v>
+        <v>57.13</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>137.49</v>
+        <v>32.13</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>101.38</v>
+        <v>20.19</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>75.05</v>
+        <v>16.79</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>276.44</v>
+        <v>95.05</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3" t="n">
-        <v>8.89</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>5.52</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>5.08</v>
-      </c>
-      <c r="E7" s="3" t="n">
-        <v>4.01</v>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>2.55</v>
-      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>80.63</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>42.1</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>42.94</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>46.17</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>159.74</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>63.81</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>69.57</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>328.88</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>32.94</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>267.07</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>140.01</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>102.48</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>74.21</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>532.4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -735,9 +1034,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,7 +1223,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -950,8 +1249,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1135,7 +1434,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1319,7 +1618,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,7 +1802,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1687,7 +1986,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1871,7 +2170,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>